<commit_message>
Updated examples for version 19.4
</commit_message>
<xml_diff>
--- a/Examples/Data/01_SourceDirectory/ThreadedCommentsSample.xlsx
+++ b/Examples/Data/01_SourceDirectory/ThreadedCommentsSample.xlsx
@@ -1,72 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DotNet Projects\Aspose\Official\Aspose_Cells_NET\Examples\Data\01_SourceDirectory\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF63A4AF-CFA8-4DCC-95A8-6F37CB77DD21}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="13410" windowHeight="11520"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={C18D8B9E-7CC1-45B4-876B-49C3FB10797E}</author>
+    <author>tc={e6157db2-d9e0-470b-bcb5-c70778e58cef}</author>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{E6157DB2-D9E0-470B-BCB5-C70778E58CEF}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    another coment from excel 365 is placed here</t>
-        </r>
+    Test Threaded Comment</t>
       </text>
     </comment>
   </commentList>
 </comments>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Comments</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -110,7 +88,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Aspose" id="{CAB98F87-B615-4D82-B758-820531BD1995}" userId="Aspose" providerId="S - 1 - 5 - 21 - 1111100000 - 1111100000 - 1111100000 - 1100"/>
+  <person displayName="Aspose Test" id="{449D05AD-E9F8-483E-BB7E-844F2212B43C}" userId="" providerId=""/>
 </personList>
 </file>
 
@@ -131,7 +109,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -143,7 +121,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -160,9 +138,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -190,14 +168,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -225,6 +220,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -375,194 +387,28 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComments1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="I4" dT="2019-01-23T07:59:25.95" personId="{CAB98F87-B615-4D82-B758-820531BD1995}" id="{C18D8B9E-7CC1-45B4-876B-49C3FB10797E}">
+  <threadedComment ref="A1" dT="2019-05-15T12:46:23.49" personId="{449D05AD-E9F8-483E-BB7E-844F2212B43C}" id="{E6157DB2-D9E0-470B-BCB5-C70778E58CEF}">
     <text>Test Threaded Comment</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I4" t="s">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Unknown Document Type" ma:contentTypeID="0x010104" ma:contentTypeVersion="0" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="05d83ceaa0bbd2e3bc716e6e66bd857a">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b3d69fe45253d5ff147bb69036b756a7">
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all/>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type" ma:readOnly="true"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="3" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C986C7B-AFF4-426A-8140-0BE06A41DA37}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2FBF48E-139C-49C2-B2F8-A8EDBB4218BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30E528BB-9A8E-459F-B923-84795C4A84F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>